<commit_message>
Spinal Engines for SOS2 업데이트 $
#959
</commit_message>
<xml_diff>
--- a/Data/Spinal Engines for SOS2 - 3254564110/3254564110.xlsx
+++ b/Data/Spinal Engines for SOS2 - 3254564110/3254564110.xlsx
@@ -5,22 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Spinal Engines for SOS2 - 3254564110\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.6\Spinal Engines for SOS2 - 3254564110\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC78C84-23E9-451F-9965-64A4F91E9349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E3B020-AB62-4BD4-826F-675733146E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240601" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240602" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -244,6 +257,94 @@
     <t>The very first part of a spinal engine. Connect this to one or more fuel engine support middle segments, then to the fuel support end</t>
   </si>
   <si>
+    <t>Keyed+SoS.SpinalEngines.FuelRate</t>
+  </si>
+  <si>
+    <t>Keyed</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.FuelRate</t>
+  </si>
+  <si>
+    <t>Fuel burn rate per second: {0} of {1} supported</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.Thrust</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.Thrust</t>
+  </si>
+  <si>
+    <t>Thrust: {0}</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.NoAccelerator</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.NoAccelerator</t>
+  </si>
+  <si>
+    <t>No engine accelerators found attached to engine!</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.NoFuelSupport</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.NoFuelSupport</t>
+  </si>
+  <si>
+    <t>No fuel support infrastructure found; Ensure accelerators are connected directly into the fuel support end!</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.NoFuelSupportEnd</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.NoFuelSupportEnd</t>
+  </si>
+  <si>
+    <t>Fuel infrastructure found, but not a complete set: Is the end missing?</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.InSufficientFuelSupport</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.InSufficientFuelSupport</t>
+  </si>
+  <si>
+    <t>Insufficent fuel structures to support accelerators: Requires {0} fuel/second, can supply {1} per second</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.DefaultError</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.DefaultError</t>
+  </si>
+  <si>
+    <t>Spinal engine isn't fully formed! Check for engine accelerators, and all three components of the fuel infrastructure!</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.BackwardsSpinal</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.BackwardsSpinal</t>
+  </si>
+  <si>
+    <t>Backwards spinal component found!</t>
+  </si>
+  <si>
+    <t>Keyed+SoS.SpinalEngines.ComponentRemoved</t>
+  </si>
+  <si>
+    <t>SoS.SpinalEngines.ComponentRemoved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A supporting {0} of the spinal engine was removed! </t>
+  </si>
+  <si>
+    <t>형상과 구조를 고려하면 이 모드의 Fuel Support는 Accumulator를 묘사한 것으로 보임. 해당 기능을 나타내기 위한 단어로써 蓄推機를 사용.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>초월공학 가속기</t>
   </si>
   <si>
@@ -253,84 +354,100 @@
     <t>대형 함선 엔진</t>
   </si>
   <si>
+    <t>대형 함선에서만 볼 수 있는 중축 엔진을 건설합니다.</t>
+  </si>
+  <si>
+    <t>인간 기술의 한계에 도달하는 더 강력한 중축 엔진을 건설합니다.</t>
+  </si>
+  <si>
+    <t>연료 가속을 위해 인간의 이해를 넘어선 물질인 이종 입자를 활용합니다.</t>
+  </si>
+  <si>
     <t>중축 엔진: 화학연료 추진기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>화학연료를 사용하는 중축 엔진입니다. 가동을 위해선 가속기와 연료 축퇴기가 필요하며, 행성간 여행에는 적합하지 않습니다.\n\n추력: 기본 2000 + 가속기당 25% 추가\n연료 소비: 화학연료 초당 4 + 가속기에 따라 추가 소비</t>
   </si>
   <si>
     <t>중축 엔진: 핵연료 추진기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>핵연료를 사용하는 중축 엔진입니다. 가동을 위해선 가속기와 연료 축퇴기가 필요하며, 행성간 여행에는 적합하지 않습니다.\n\n추력: 기본 2500 + 가속기당 25% 추가\n연료 소비: 우라늄 연료 초당 3 + 가속기에 따라 추가 소비</t>
   </si>
   <si>
     <t>중축 엔진: 가속기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연료를 연소 시점에 앞서 가속합니다. 하나 이상의 가속기를 연료 축퇴기의 연결부에 연결한 다음, 추진기를 장착하여 엔진을 구성합니다.\n\n기본 추력을 25% 증가시키지만, 연료 소비도 25% 늘어납니다.\n\n가속기를 중축할수록 더 큰 연료 축퇴 기관이 필요하며, 전력 소모도 미세하게 증가합니다.</t>
+  </si>
+  <si>
+    <t>중축 엔진: 고효율 가속기</t>
+  </si>
+  <si>
+    <t>상당한 전력을 소비하여 연료를 연소 시점에 앞서 가속합니다. 하나 이상의 가속기를 연료 축퇴기의 연결부에 연결한 다음, 추진기를 장착하여 엔진을 구성합니다.\n\n기본 추력을 25% 증가시키지만, 연료 소비도 5% 늘어납니다.\n\n가속기를 중축할수록 더 큰 연료 축퇴 기관이 필요하며, 전력 소모도 크게 증가합니다. 이 고효율 모델은 연비가 개선되어 축퇴기 용량을 적게 차지하지만, 일반적인 가속기보다 많은 전력을 소모합니다.</t>
   </si>
   <si>
     <t>중축 엔진: 초월공학 가속기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이종 역장을 활용하여 연료를 연소 시점에 앞서 가속합니다. 하나 이상의 가속기를 연료 축퇴기의 연결부에 연결한 다음, 추진기를 장착하여 엔진을 구성합니다.\n\n기본 추력을 25% 증가시키지만, 연료 소비도 1% 늘어납니다.\n\n이 가속기는 매우 작은 축퇴기로도 끝없이 중축할 수 있을 정도로 효율이 뛰어나지만, 작동에 엄청난 양의 전력이 필요합니다.</t>
+  </si>
+  <si>
+    <t>중축 엔진: 연료 축퇴기 연결부</t>
+  </si>
+  <si>
+    <t>연료 축퇴 기관의 마지막 부분입니다.\n\n이 부분을 통하여 연료 축퇴기와 가속기를 연결합니다.</t>
   </si>
   <si>
     <t>중축 엔진: 연료 축퇴기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>대형 함선에서만 볼 수 있는 중축 엔진을 건설합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중축 엔진: 고효율 가속기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>형상과 구조를 고려하면 이 모드의 Fuel Support는 Accumulator를 묘사한 것으로 보임. 해당 기능을 나타내기 위한 단어로써 蓄推機를 사용.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간 기술의 한계에 도달하는 더 강력한 중축 엔진을 건설합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>연료 가속을 위해 인간의 이해를 넘어선 물질인 이종 입자를 활용합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중축 엔진: 연료 축퇴기 연결부</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연료 축퇴 기관의 중축 부분입니다. 각각의 축퇴기는 표준적인 엔진 가속기 3개가 추가적으로 증가시키는 연료 소모율을 감당할 수 있습니다.\n\n연료 축퇴기 상단과 연결부 사이에 필요한 만큼 구축하세요.</t>
   </si>
   <si>
     <t>중축 엔진: 연료 축퇴기 상부</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>연료 축퇴 기관의 중축 부분입니다. 각각의 축퇴기는 표준적인 엔진 가속기 3개가 추가적으로 증가시키는 연료 소모율을 감당할 수 있습니다.\n\n연료 축퇴기 상단과 연결부 사이에 필요한 만큼 구축하세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>화학연료를 사용하는 중축 엔진입니다. 가동을 위해선 가속기와 연료 축퇴기가 필요하며, 행성간 여행에는 적합하지 않습니다.\n\n추력: 기본 2000 + 가속기당 25% 추가\n연료 소비: 화학연료 초당 4 + 가속기에 따라 추가 소비</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>핵연료를 사용하는 중축 엔진입니다. 가동을 위해선 가속기와 연료 축퇴기가 필요하며, 행성간 여행에는 적합하지 않습니다.\n\n추력: 기본 2500 + 가속기당 25% 추가\n연료 소비: 우라늄 연료 초당 3 + 가속기에 따라 추가 소비</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>연료를 연소 시점에 앞서 가속합니다. 하나 이상의 가속기를 연료 축퇴기의 연결부에 연결한 다음, 추진기를 장착하여 엔진을 구성합니다.\n\n기본 추력을 25% 증가시키지만, 연료 소비도 25% 늘어납니다.\n\n가속기를 중축할수록 더 큰 연료 축퇴 기관이 필요하며, 전력 소모도 미세하게 증가합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>상당한 전력을 소비하여 연료를 연소 시점에 앞서 가속합니다. 하나 이상의 가속기를 연료 축퇴기의 연결부에 연결한 다음, 추진기를 장착하여 엔진을 구성합니다.\n\n기본 추력을 25% 증가시키지만, 연료 소비도 5% 늘어납니다.\n\n가속기를 중축할수록 더 큰 연료 축퇴 기관이 필요하며, 전력 소모도 크게 증가합니다. 이 고효율 모델은 연비가 개선되어 축퇴기 용량을 적게 차지하지만, 일반적인 가속기보다 많은 전력을 소모합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이종 역장을 활용하여 연료를 연소 시점에 앞서 가속합니다. 하나 이상의 가속기를 연료 축퇴기의 연결부에 연결한 다음, 추진기를 장착하여 엔진을 구성합니다.\n\n기본 추력을 25% 증가시키지만, 연료 소비도 1% 늘어납니다.\n\n이 가속기는 매우 작은 축퇴기로도 끝없이 중축할 수 있을 정도로 효율이 뛰어나지만, 작동에 엄청난 양의 전력이 필요합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>연료 축퇴 기관의 마지막 부분입니다.\n\n이 부분을 통하여 연료 축퇴기와 가속기를 연결합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>연료 축퇴 기관의 첫 번째 부분입니다.\n\n이 부분을 연료 축퇴기에 연결하여 중축 엔진의 시작점을 구축하세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>추력: {0}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>초당 연료 소모율/축퇴기 용량: {0}/{1}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: 엔진 가속기가 없습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: 연료 축퇴기가 없습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: 연료 축퇴기가 완전하지 않습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: 축퇴기 용량이 부족합니다.\n요구량/가용량: {0}/{1}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: 엔진이 완성되지 않았습니다.\n추진기, 가속기, 축퇴기가 모두 구성돼있는지 확인하세요.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: 방향이 반대로 설치된 부품이 있습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작동 불가: {0}(이)가 제거되었습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -351,16 +468,16 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -402,7 +519,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -713,21 +830,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="54.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="143.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="127.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="136.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -765,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -782,7 +899,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -799,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -816,7 +933,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -833,7 +950,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -850,7 +967,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -867,7 +984,7 @@
         <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -884,7 +1001,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -901,7 +1018,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -918,7 +1035,7 @@
         <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -935,7 +1052,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -952,7 +1069,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -969,7 +1086,7 @@
         <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -986,7 +1103,7 @@
         <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -1003,7 +1120,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1020,7 +1137,7 @@
         <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -1037,10 +1154,10 @@
         <v>58</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1057,7 +1174,7 @@
         <v>61</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1074,7 +1191,7 @@
         <v>64</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1091,7 +1208,7 @@
         <v>67</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1108,7 +1225,7 @@
         <v>70</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -1125,11 +1242,164 @@
         <v>73</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>